<commit_message>
Adição de loop ao chamar o metodo que trata o popUp, criação de uma classe para ficar com os relatorios
</commit_message>
<xml_diff>
--- a/Planilha modelo.xlsx
+++ b/Planilha modelo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="72">
   <si>
     <t>senha</t>
   </si>
@@ -735,7 +735,7 @@
       <c r="O2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="0"/>
+      <c r="AD2"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
@@ -778,7 +778,7 @@
       <c r="O3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="0"/>
+      <c r="AD3"/>
     </row>
     <row r="4">
       <c r="A4" s="16"/>

</xml_diff>